<commit_message>
Updating the Quiz Bank
</commit_message>
<xml_diff>
--- a/Deployment/TeamsQuestionBank.xlsx
+++ b/Deployment/TeamsQuestionBank.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swarora\Desktop\Deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757A6A4D-F9D8-4EDA-A3C6-3FEBF1A0114D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48245286-2D00-4644-BF41-43CD5A884DA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{0033BA41-4B9D-490C-9F50-957A435A7F98}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="258">
   <si>
     <t>Question</t>
   </si>
@@ -823,6 +823,12 @@
   </si>
   <si>
     <t>S.No</t>
+  </si>
+  <si>
+    <t>Can't Say</t>
+  </si>
+  <si>
+    <t>None of the Above</t>
   </si>
 </sst>
 </file>
@@ -1327,7 +1333,7 @@
   <dimension ref="A1:G78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,8 +1636,12 @@
       <c r="D13" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
+      <c r="E13" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>257</v>
+      </c>
       <c r="G13" s="10" t="b">
         <v>0</v>
       </c>
@@ -1672,8 +1682,12 @@
       <c r="D15" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
+      <c r="E15" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>257</v>
+      </c>
       <c r="G15" s="10" t="b">
         <v>0</v>
       </c>
@@ -1852,6 +1866,12 @@
       <c r="D23" s="12" t="s">
         <v>67</v>
       </c>
+      <c r="E23" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>257</v>
+      </c>
       <c r="G23" s="12" t="s">
         <v>66</v>
       </c>
@@ -1869,6 +1889,12 @@
       <c r="D24" s="12" t="s">
         <v>67</v>
       </c>
+      <c r="E24" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>257</v>
+      </c>
       <c r="G24" s="12" t="s">
         <v>67</v>
       </c>
@@ -1932,6 +1958,12 @@
       <c r="D27" s="12" t="s">
         <v>67</v>
       </c>
+      <c r="E27" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>257</v>
+      </c>
       <c r="G27" s="12" t="s">
         <v>67</v>
       </c>
@@ -2081,8 +2113,12 @@
       <c r="D34" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
+      <c r="E34" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>257</v>
+      </c>
       <c r="G34" s="13" t="b">
         <v>0</v>
       </c>
@@ -2192,8 +2228,12 @@
       <c r="D39" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
+      <c r="E39" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>257</v>
+      </c>
       <c r="G39" s="10" t="b">
         <v>0</v>
       </c>
@@ -2211,8 +2251,12 @@
       <c r="D40" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
+      <c r="E40" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>257</v>
+      </c>
       <c r="G40" s="10" t="s">
         <v>66</v>
       </c>
@@ -2345,8 +2389,12 @@
       <c r="D46" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
+      <c r="E46" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>257</v>
+      </c>
       <c r="G46" s="9" t="s">
         <v>66</v>
       </c>
@@ -2364,8 +2412,12 @@
       <c r="D47" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
+      <c r="E47" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>257</v>
+      </c>
       <c r="G47" s="15" t="s">
         <v>66</v>
       </c>
@@ -2429,6 +2481,12 @@
       <c r="D50" s="12" t="b">
         <v>0</v>
       </c>
+      <c r="E50" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>257</v>
+      </c>
       <c r="G50" s="12" t="b">
         <v>0</v>
       </c>
@@ -2446,6 +2504,12 @@
       <c r="D51" s="12" t="b">
         <v>0</v>
       </c>
+      <c r="E51" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>257</v>
+      </c>
       <c r="G51" s="12" t="b">
         <v>1</v>
       </c>
@@ -2486,6 +2550,12 @@
       <c r="D53" s="12" t="b">
         <v>0</v>
       </c>
+      <c r="E53" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="F53" s="12" t="s">
+        <v>257</v>
+      </c>
       <c r="G53" s="12" t="b">
         <v>1</v>
       </c>
@@ -2618,8 +2688,12 @@
       <c r="D59" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8"/>
+      <c r="E59" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="G59" s="8" t="b">
         <v>0</v>
       </c>
@@ -2821,6 +2895,12 @@
       <c r="D68" s="12" t="b">
         <v>0</v>
       </c>
+      <c r="E68" t="s">
+        <v>256</v>
+      </c>
+      <c r="F68" t="s">
+        <v>257</v>
+      </c>
       <c r="G68" s="12" t="b">
         <v>1</v>
       </c>
@@ -2838,10 +2918,10 @@
       <c r="D69" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="E69" s="12" t="s">
+      <c r="E69" t="s">
         <v>223</v>
       </c>
-      <c r="F69" s="12" t="s">
+      <c r="F69" t="s">
         <v>221</v>
       </c>
       <c r="G69" s="12" t="s">
@@ -2861,6 +2941,12 @@
       <c r="D70" s="12" t="b">
         <v>0</v>
       </c>
+      <c r="E70" t="s">
+        <v>256</v>
+      </c>
+      <c r="F70" t="s">
+        <v>257</v>
+      </c>
       <c r="G70" s="12" t="b">
         <v>1</v>
       </c>
@@ -2878,6 +2964,12 @@
       <c r="D71" s="12" t="b">
         <v>0</v>
       </c>
+      <c r="E71" t="s">
+        <v>256</v>
+      </c>
+      <c r="F71" t="s">
+        <v>257</v>
+      </c>
       <c r="G71" s="12" t="b">
         <v>0</v>
       </c>
@@ -2895,10 +2987,10 @@
       <c r="D72" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="E72" s="12" t="s">
+      <c r="E72" t="s">
         <v>230</v>
       </c>
-      <c r="F72" s="12" t="s">
+      <c r="F72" t="s">
         <v>231</v>
       </c>
       <c r="G72" s="12" t="s">
@@ -2918,6 +3010,12 @@
       <c r="D73" s="12" t="b">
         <v>0</v>
       </c>
+      <c r="E73" t="s">
+        <v>256</v>
+      </c>
+      <c r="F73" t="s">
+        <v>257</v>
+      </c>
       <c r="G73" s="12" t="b">
         <v>1</v>
       </c>
@@ -2935,6 +3033,12 @@
       <c r="D74" s="12" t="b">
         <v>0</v>
       </c>
+      <c r="E74" t="s">
+        <v>256</v>
+      </c>
+      <c r="F74" t="s">
+        <v>257</v>
+      </c>
       <c r="G74" s="12" t="b">
         <v>1</v>
       </c>
@@ -2952,10 +3056,10 @@
       <c r="D75" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="E75" s="12" t="s">
+      <c r="E75" t="s">
         <v>236</v>
       </c>
-      <c r="F75" s="12" t="s">
+      <c r="F75" t="s">
         <v>237</v>
       </c>
       <c r="G75" s="12" t="s">
@@ -2975,6 +3079,12 @@
       <c r="D76" s="12" t="b">
         <v>0</v>
       </c>
+      <c r="E76" t="s">
+        <v>256</v>
+      </c>
+      <c r="F76" t="s">
+        <v>257</v>
+      </c>
       <c r="G76" s="12" t="b">
         <v>1</v>
       </c>
@@ -2992,10 +3102,10 @@
       <c r="D77" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="E77" s="12" t="s">
+      <c r="E77" t="s">
         <v>243</v>
       </c>
-      <c r="F77" s="12" t="s">
+      <c r="F77" t="s">
         <v>244</v>
       </c>
       <c r="G77" s="12" t="s">
@@ -3015,10 +3125,10 @@
       <c r="D78" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="E78" s="12" t="s">
+      <c r="E78" t="s">
         <v>248</v>
       </c>
-      <c r="F78" s="12" t="s">
+      <c r="F78" t="s">
         <v>249</v>
       </c>
       <c r="G78" s="12" t="s">
@@ -3277,18 +3387,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3311,14 +3421,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBB43C29-2953-4FA1-9CDF-73853D523B4C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03E74EDC-EB10-4BFD-841D-D40F0AB415C3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="d5eecfe1-67dc-47ad-91d3-ebcc6aa3a458"/>
@@ -3333,4 +3435,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBB43C29-2953-4FA1-9CDF-73853D523B4C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated Teams Ques bank
</commit_message>
<xml_diff>
--- a/Deployment/TeamsQuestionBank.xlsx
+++ b/Deployment/TeamsQuestionBank.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swarora\Desktop\Deployment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swarora\QuizApp\Deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48245286-2D00-4644-BF41-43CD5A884DA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D488B2-69B8-4E8C-A262-5F498B6FBDCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{0033BA41-4B9D-490C-9F50-957A435A7F98}"/>
   </bookViews>
@@ -822,13 +822,13 @@
     <t>Answer</t>
   </si>
   <si>
-    <t>S.No</t>
-  </si>
-  <si>
     <t>Can't Say</t>
   </si>
   <si>
     <t>None of the Above</t>
+  </si>
+  <si>
+    <t>SNo.</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +1007,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE074867-A302-45CB-A2F3-6F109B7527C5}" name="Table1" displayName="Table1" ref="A1:G78" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:G78" xr:uid="{41955F9D-CA80-48C2-B8E5-364BCE8B0788}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3C9A1044-704C-47FF-8C54-B922818E1B47}" name="S.No"/>
+    <tableColumn id="1" xr3:uid="{3C9A1044-704C-47FF-8C54-B922818E1B47}" name="SNo."/>
     <tableColumn id="2" xr3:uid="{A9D40C83-9864-4C7F-B838-6567C86F05DF}" name="Question"/>
     <tableColumn id="3" xr3:uid="{EEE6ACE9-DB51-478B-8D6C-3EC6FC3D7046}" name="Option1" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{54AFF299-ED2C-4787-9557-42848FC4209E}" name="Option2" dataDxfId="3"/>
@@ -1333,7 +1333,7 @@
   <dimension ref="A1:G78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,7 +1349,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1637,10 +1637,10 @@
         <v>0</v>
       </c>
       <c r="E13" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>256</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>257</v>
       </c>
       <c r="G13" s="10" t="b">
         <v>0</v>
@@ -1683,10 +1683,10 @@
         <v>0</v>
       </c>
       <c r="E15" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>256</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>257</v>
       </c>
       <c r="G15" s="10" t="b">
         <v>0</v>
@@ -1867,10 +1867,10 @@
         <v>67</v>
       </c>
       <c r="E23" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="F23" s="12" t="s">
         <v>256</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>257</v>
       </c>
       <c r="G23" s="12" t="s">
         <v>66</v>
@@ -1890,10 +1890,10 @@
         <v>67</v>
       </c>
       <c r="E24" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="F24" s="12" t="s">
         <v>256</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>257</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>67</v>
@@ -1959,10 +1959,10 @@
         <v>67</v>
       </c>
       <c r="E27" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="F27" s="12" t="s">
         <v>256</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>257</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>67</v>
@@ -2114,10 +2114,10 @@
         <v>1</v>
       </c>
       <c r="E34" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="F34" s="13" t="s">
         <v>256</v>
-      </c>
-      <c r="F34" s="13" t="s">
-        <v>257</v>
       </c>
       <c r="G34" s="13" t="b">
         <v>0</v>
@@ -2229,10 +2229,10 @@
         <v>0</v>
       </c>
       <c r="E39" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="F39" s="10" t="s">
         <v>256</v>
-      </c>
-      <c r="F39" s="10" t="s">
-        <v>257</v>
       </c>
       <c r="G39" s="10" t="b">
         <v>0</v>
@@ -2252,10 +2252,10 @@
         <v>67</v>
       </c>
       <c r="E40" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="F40" s="10" t="s">
         <v>256</v>
-      </c>
-      <c r="F40" s="10" t="s">
-        <v>257</v>
       </c>
       <c r="G40" s="10" t="s">
         <v>66</v>
@@ -2390,10 +2390,10 @@
         <v>67</v>
       </c>
       <c r="E46" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="F46" s="15" t="s">
         <v>256</v>
-      </c>
-      <c r="F46" s="15" t="s">
-        <v>257</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>66</v>
@@ -2413,10 +2413,10 @@
         <v>67</v>
       </c>
       <c r="E47" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="F47" s="15" t="s">
         <v>256</v>
-      </c>
-      <c r="F47" s="15" t="s">
-        <v>257</v>
       </c>
       <c r="G47" s="15" t="s">
         <v>66</v>
@@ -2482,10 +2482,10 @@
         <v>0</v>
       </c>
       <c r="E50" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="F50" s="12" t="s">
         <v>256</v>
-      </c>
-      <c r="F50" s="12" t="s">
-        <v>257</v>
       </c>
       <c r="G50" s="12" t="b">
         <v>0</v>
@@ -2505,10 +2505,10 @@
         <v>0</v>
       </c>
       <c r="E51" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="F51" s="12" t="s">
         <v>256</v>
-      </c>
-      <c r="F51" s="12" t="s">
-        <v>257</v>
       </c>
       <c r="G51" s="12" t="b">
         <v>1</v>
@@ -2551,10 +2551,10 @@
         <v>0</v>
       </c>
       <c r="E53" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="F53" s="12" t="s">
         <v>256</v>
-      </c>
-      <c r="F53" s="12" t="s">
-        <v>257</v>
       </c>
       <c r="G53" s="12" t="b">
         <v>1</v>
@@ -2689,10 +2689,10 @@
         <v>0</v>
       </c>
       <c r="E59" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="F59" s="8" t="s">
         <v>256</v>
-      </c>
-      <c r="F59" s="8" t="s">
-        <v>257</v>
       </c>
       <c r="G59" s="8" t="b">
         <v>0</v>
@@ -2896,10 +2896,10 @@
         <v>0</v>
       </c>
       <c r="E68" t="s">
+        <v>255</v>
+      </c>
+      <c r="F68" t="s">
         <v>256</v>
-      </c>
-      <c r="F68" t="s">
-        <v>257</v>
       </c>
       <c r="G68" s="12" t="b">
         <v>1</v>
@@ -2942,10 +2942,10 @@
         <v>0</v>
       </c>
       <c r="E70" t="s">
+        <v>255</v>
+      </c>
+      <c r="F70" t="s">
         <v>256</v>
-      </c>
-      <c r="F70" t="s">
-        <v>257</v>
       </c>
       <c r="G70" s="12" t="b">
         <v>1</v>
@@ -2965,10 +2965,10 @@
         <v>0</v>
       </c>
       <c r="E71" t="s">
+        <v>255</v>
+      </c>
+      <c r="F71" t="s">
         <v>256</v>
-      </c>
-      <c r="F71" t="s">
-        <v>257</v>
       </c>
       <c r="G71" s="12" t="b">
         <v>0</v>
@@ -3011,10 +3011,10 @@
         <v>0</v>
       </c>
       <c r="E73" t="s">
+        <v>255</v>
+      </c>
+      <c r="F73" t="s">
         <v>256</v>
-      </c>
-      <c r="F73" t="s">
-        <v>257</v>
       </c>
       <c r="G73" s="12" t="b">
         <v>1</v>
@@ -3034,10 +3034,10 @@
         <v>0</v>
       </c>
       <c r="E74" t="s">
+        <v>255</v>
+      </c>
+      <c r="F74" t="s">
         <v>256</v>
-      </c>
-      <c r="F74" t="s">
-        <v>257</v>
       </c>
       <c r="G74" s="12" t="b">
         <v>1</v>
@@ -3080,10 +3080,10 @@
         <v>0</v>
       </c>
       <c r="E76" t="s">
+        <v>255</v>
+      </c>
+      <c r="F76" t="s">
         <v>256</v>
-      </c>
-      <c r="F76" t="s">
-        <v>257</v>
       </c>
       <c r="G76" s="12" t="b">
         <v>1</v>
@@ -3170,6 +3170,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A00D9453AFA9EC4B9022F8FD60023C27" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7f2cdc1227837d630307acdf483fde50">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0e0f4575-6a25-48ed-8a9c-18fd8239b097" xmlns:ns3="d5eecfe1-67dc-47ad-91d3-ebcc6aa3a458" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b471ff19f16803ee6b380916ee2a217a" ns2:_="" ns3:_="">
     <xsd:import namespace="0e0f4575-6a25-48ed-8a9c-18fd8239b097"/>
@@ -3386,12 +3392,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3402,6 +3402,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03E74EDC-EB10-4BFD-841D-D40F0AB415C3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="d5eecfe1-67dc-47ad-91d3-ebcc6aa3a458"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="0e0f4575-6a25-48ed-8a9c-18fd8239b097"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61906E0A-D393-4883-B3B1-60864BB5178D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3420,23 +3437,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03E74EDC-EB10-4BFD-841D-D40F0AB415C3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="d5eecfe1-67dc-47ad-91d3-ebcc6aa3a458"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="0e0f4575-6a25-48ed-8a9c-18fd8239b097"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBB43C29-2953-4FA1-9CDF-73853D523B4C}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Commiting changes to Teams Ques bank
</commit_message>
<xml_diff>
--- a/Deployment/TeamsQuestionBank.xlsx
+++ b/Deployment/TeamsQuestionBank.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swarora\QuizApp\Deployment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swarora\Desktop\Deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D488B2-69B8-4E8C-A262-5F498B6FBDCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48245286-2D00-4644-BF41-43CD5A884DA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{0033BA41-4B9D-490C-9F50-957A435A7F98}"/>
   </bookViews>
@@ -822,13 +822,13 @@
     <t>Answer</t>
   </si>
   <si>
+    <t>S.No</t>
+  </si>
+  <si>
     <t>Can't Say</t>
   </si>
   <si>
     <t>None of the Above</t>
-  </si>
-  <si>
-    <t>SNo.</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +1007,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE074867-A302-45CB-A2F3-6F109B7527C5}" name="Table1" displayName="Table1" ref="A1:G78" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:G78" xr:uid="{41955F9D-CA80-48C2-B8E5-364BCE8B0788}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3C9A1044-704C-47FF-8C54-B922818E1B47}" name="SNo."/>
+    <tableColumn id="1" xr3:uid="{3C9A1044-704C-47FF-8C54-B922818E1B47}" name="S.No"/>
     <tableColumn id="2" xr3:uid="{A9D40C83-9864-4C7F-B838-6567C86F05DF}" name="Question"/>
     <tableColumn id="3" xr3:uid="{EEE6ACE9-DB51-478B-8D6C-3EC6FC3D7046}" name="Option1" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{54AFF299-ED2C-4787-9557-42848FC4209E}" name="Option2" dataDxfId="3"/>
@@ -1333,7 +1333,7 @@
   <dimension ref="A1:G78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,7 +1349,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1637,10 +1637,10 @@
         <v>0</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G13" s="10" t="b">
         <v>0</v>
@@ -1683,10 +1683,10 @@
         <v>0</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G15" s="10" t="b">
         <v>0</v>
@@ -1867,10 +1867,10 @@
         <v>67</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G23" s="12" t="s">
         <v>66</v>
@@ -1890,10 +1890,10 @@
         <v>67</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>67</v>
@@ -1959,10 +1959,10 @@
         <v>67</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>67</v>
@@ -2114,10 +2114,10 @@
         <v>1</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G34" s="13" t="b">
         <v>0</v>
@@ -2229,10 +2229,10 @@
         <v>0</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G39" s="10" t="b">
         <v>0</v>
@@ -2252,10 +2252,10 @@
         <v>67</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G40" s="10" t="s">
         <v>66</v>
@@ -2390,10 +2390,10 @@
         <v>67</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>66</v>
@@ -2413,10 +2413,10 @@
         <v>67</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G47" s="15" t="s">
         <v>66</v>
@@ -2482,10 +2482,10 @@
         <v>0</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G50" s="12" t="b">
         <v>0</v>
@@ -2505,10 +2505,10 @@
         <v>0</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G51" s="12" t="b">
         <v>1</v>
@@ -2551,10 +2551,10 @@
         <v>0</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F53" s="12" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G53" s="12" t="b">
         <v>1</v>
@@ -2689,10 +2689,10 @@
         <v>0</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G59" s="8" t="b">
         <v>0</v>
@@ -2896,10 +2896,10 @@
         <v>0</v>
       </c>
       <c r="E68" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F68" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G68" s="12" t="b">
         <v>1</v>
@@ -2942,10 +2942,10 @@
         <v>0</v>
       </c>
       <c r="E70" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F70" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G70" s="12" t="b">
         <v>1</v>
@@ -2965,10 +2965,10 @@
         <v>0</v>
       </c>
       <c r="E71" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F71" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G71" s="12" t="b">
         <v>0</v>
@@ -3011,10 +3011,10 @@
         <v>0</v>
       </c>
       <c r="E73" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F73" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G73" s="12" t="b">
         <v>1</v>
@@ -3034,10 +3034,10 @@
         <v>0</v>
       </c>
       <c r="E74" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F74" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G74" s="12" t="b">
         <v>1</v>
@@ -3080,10 +3080,10 @@
         <v>0</v>
       </c>
       <c r="E76" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F76" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G76" s="12" t="b">
         <v>1</v>
@@ -3170,12 +3170,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A00D9453AFA9EC4B9022F8FD60023C27" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7f2cdc1227837d630307acdf483fde50">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0e0f4575-6a25-48ed-8a9c-18fd8239b097" xmlns:ns3="d5eecfe1-67dc-47ad-91d3-ebcc6aa3a458" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b471ff19f16803ee6b380916ee2a217a" ns2:_="" ns3:_="">
     <xsd:import namespace="0e0f4575-6a25-48ed-8a9c-18fd8239b097"/>
@@ -3392,6 +3386,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3402,23 +3402,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03E74EDC-EB10-4BFD-841D-D40F0AB415C3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="d5eecfe1-67dc-47ad-91d3-ebcc6aa3a458"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="0e0f4575-6a25-48ed-8a9c-18fd8239b097"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61906E0A-D393-4883-B3B1-60864BB5178D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3437,6 +3420,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03E74EDC-EB10-4BFD-841D-D40F0AB415C3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="d5eecfe1-67dc-47ad-91d3-ebcc6aa3a458"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="0e0f4575-6a25-48ed-8a9c-18fd8239b097"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBB43C29-2953-4FA1-9CDF-73853D523B4C}">
   <ds:schemaRefs>

</xml_diff>